<commit_message>
feat: still acoppling the generate.py
</commit_message>
<xml_diff>
--- a/djangoproyect/static/requests/emulation/requests_database.xlsx
+++ b/djangoproyect/static/requests/emulation/requests_database.xlsx
@@ -1,62 +1,55 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="4">
     <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -64,45 +57,97 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -213,24 +258,100 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A2:A11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetData>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>document</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>applicant</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>manager</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>initial_date</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>final_date</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>past_days</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  <pageSetup orientation="portrait" paperSize="1" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="1" useFirstPageNumber="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentOddEven="0" differentFirst="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: create partial correct
</commit_message>
<xml_diff>
--- a/djangoproyect/static/requests/emulation/requests_database.xlsx
+++ b/djangoproyect/static/requests/emulation/requests_database.xlsx
@@ -16,7 +16,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="6">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="166" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="167" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="168" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="169" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="4">
     <font>
       <name val="Arial"/>
@@ -67,10 +74,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -259,99 +275,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:A11"/>
+  <dimension ref="A2:V3"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>document</t>
-        </is>
-      </c>
+          <t>sit.numbers</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>jonathan89</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>blackwelltristan</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>45364</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>45365</v>
+      </c>
+      <c r="F2" t="n">
+        <v>13</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Worker realize stop region. Beyond machine wonder appear artist mind pass. Us or always wear.
+Form recent central have here eye. Building tonight them beat movement other window.</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Charles Anderson</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Type 1</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>wayne10,smithtyler</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>applicant</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>manager</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>initial_date</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>final_date</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>past_days</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>status</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>title</t>
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>expert.tiff</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>matthewdelacruz</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>blackwelltristan</t>
+        </is>
+      </c>
+      <c r="O3" s="5" t="n">
+        <v>45356</v>
+      </c>
+      <c r="P3" s="5" t="n">
+        <v>45363</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>21</v>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Keep pass small figure many box. Bad also field crime police close concern. Police start pull wrong.</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>Kendra Moran</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>Approved</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>Type 2</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>jonathan89,edwardjoseph,smithtyler</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup orientation="portrait" paperSize="1" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="1" useFirstPageNumber="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentOddEven="0" differentFirst="0">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: adapted the search to the sharepoint api
</commit_message>
<xml_diff>
--- a/djangoproyect/static/requests/emulation/requests_database.xlsx
+++ b/djangoproyect/static/requests/emulation/requests_database.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1017,10 +1017,10 @@
           <t>Scott Rush (@84851164)</t>
         </is>
       </c>
-      <c r="E11" s="3" t="n">
+      <c r="E11" s="2" t="n">
         <v>45367</v>
       </c>
-      <c r="F11" s="3" t="n">
+      <c r="F11" s="2" t="n">
         <v>45369</v>
       </c>
       <c r="G11" t="n">
@@ -1051,6 +1051,1104 @@
       <c r="L11" t="inlineStr">
         <is>
           <t>Heather Cruz (@55546980),Michael Jensen (@92101631),Anne Morales (@30008743)</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>just.xls</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Jessica Chavez (@67584311)</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Jessica Chavez (@67584311)</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>45370</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>45386</v>
+      </c>
+      <c r="G12" t="n">
+        <v>8</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>A tree successful art concern look but. Represent theory bad pattern second happen.</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Mrs. Shelia Flores MD</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>RECHAZADO - CENCO</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Type 3</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Kurt Valdez (@96002744),Jessica Chavez (@67584311)</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>address.pptx</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Angela Campbell (@10438660)</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Jessica Chavez (@67584311)</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>45371</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>45376</v>
+      </c>
+      <c r="G13" t="n">
+        <v>7</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Collection appear usually by last.
+Specific home language cultural.
+Note college adult those save author stand crime. Forget strong different present your. Man behavior like debate.</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Paul Allen</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>RECHAZADO - CONTABILIDAD</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Type 1</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Jessica Chavez (@67584311),Jill Caldwell (@55215677),Elizabeth Ross (@86396417)</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>safe.key</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Elizabeth Ross (@86396417)</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Elizabeth Ross (@86396417)</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>45354</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>45377</v>
+      </c>
+      <c r="G14" t="n">
+        <v>24</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Law fact small hot. Few job agreement.
+Sense national over serious watch left. Watch ten thing million.
+Election serious record series beat likely. Game type series entire three marriage media only.</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Tiffany Chapman</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>PAGADO - CONTABILIDAD</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Type 1</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Jill Caldwell (@55215677),Elizabeth Ross (@86396417),Kurt Valdez (@96002744)</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>like.flac</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Jill Caldwell (@55215677)</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Dorothy Mcclain (@57192986)</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>45361</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>45374</v>
+      </c>
+      <c r="G15" t="n">
+        <v>17</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Standard team again professor our science and. One play pretty property friend relate design.</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Katherine Brown</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>APROBADO - DECANO</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Type 3</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Kurt Valdez (@96002744)</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>call.mp3</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Kurt Valdez (@96002744)</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Linda Russell (@58176224)</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>45376</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>45386</v>
+      </c>
+      <c r="G16" t="n">
+        <v>2</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Office president bank rise debate officer. Thought significant from month stuff to interest. Throughout member ask lot.
+Item wall act mind cell baby visit job. Hand notice owner information with.</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Anthony Cervantes</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>RECHAZADO - DECANO</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Type 1</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Jessica Chavez (@67584311)</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>about.gif</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Dorothy Mcclain (@57192986)</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Kurt Valdez (@96002744)</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>45370</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>45388</v>
+      </c>
+      <c r="G17" t="n">
+        <v>8</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>School memory common can. Pm TV finally be. Always address weight capital.
+Organization clearly available ask. Employee usually require east. By actually then none.</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>John Bernard</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>APROBADO - CENCO</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Type 2</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Elizabeth Ross (@86396417)</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>eight.wav</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Bruce Jones (@79789358)</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Angela Campbell (@10438660)</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>45369</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>45383</v>
+      </c>
+      <c r="G18" t="n">
+        <v>9</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Particularly computer reason him industry here evidence. Key art bank assume single. Them produce generation even star.</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Janet Green</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>RECHAZADO - CENCO</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Type 3</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Kurt Valdez (@96002744),Elizabeth Ross (@86396417)</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>store.gif</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Elizabeth Ross (@86396417)</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Dorothy Mcclain (@57192986)</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>45369</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>45381</v>
+      </c>
+      <c r="G19" t="n">
+        <v>9</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Tree ready group figure allow hard. Either candidate speak cut road continue day letter.</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Kimberly Cervantes</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>CERRADO</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Type 2</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Elizabeth Ross (@86396417),Elizabeth Ross (@86396417)</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>her.js</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Angela Campbell (@10438660)</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Angela Campbell (@10438660)</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>45379</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>45395</v>
+      </c>
+      <c r="G20" t="n">
+        <v>-1</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>New hit building successful. Food there spend stop. Color white can both standard everybody tell live. House company success wrong school people.
+Around until church account. Idea during history.</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Christine Cain</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>APROBADO - DECANO</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Type 1</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Jill Caldwell (@55215677),Kurt Valdez (@96002744),Elizabeth Ross (@86396417)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>little.webm</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Linda Russell (@58176224)</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Wendy Gonzalez (@46065515)</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>45381</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <v>45388</v>
+      </c>
+      <c r="G21" t="n">
+        <v>-3</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Each bed house affect. Option clear information. Discussion production tell campaign state.
+Because population sense now each. Through add heavy arrive professor throughout.</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Jeffrey Berry</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>RECHAZADO - CENCO</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Type 2</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Jessica Chavez (@67584311),Jill Caldwell (@55215677),Elizabeth Ross (@86396417)</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>partner.js</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Tyler Gomez (@51016002)</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Jodi Hansen (@21049704)</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>45350</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>45375</v>
+      </c>
+      <c r="G22" t="n">
+        <v>28</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Money our weight movie part they. Window series individual nothing final. Detail official your ever television kind.</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Christina Silva</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>APROBADO - CENCO</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Type 2</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Denise Cunningham (@61472431),Juan Herrera (@12010452),Jasmine Abbott (@7142464)</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>power.json</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Jodi Hansen (@21049704)</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Michelle Sandoval (@88258637)</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>45367</v>
+      </c>
+      <c r="F23" s="2" t="n">
+        <v>45369</v>
+      </c>
+      <c r="G23" t="n">
+        <v>11</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Specific goal television home difference thousand. Quickly difficult good talk oil. Dinner film doctor important.
+Whom key firm nearly heart.</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Andrea Mercado</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>RECHAZADO - DECANO</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Type 3</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Denise Cunningham (@61472431)</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>life.ppt</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Michelle Sandoval (@88258637)</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Alexis Garza (@65251217)</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>45356</v>
+      </c>
+      <c r="F24" s="2" t="n">
+        <v>45368</v>
+      </c>
+      <c r="G24" t="n">
+        <v>22</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Design behavior rock at could decision guess. Hotel or condition success let. Dream away difficult war.
+Tv drop head finally meeting standard level.</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Brian Freeman</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>RECHAZADO - CONTABILIDAD</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Type 2</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>Jonathan Hall (@81435130),Juan Herrera (@12010452)</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>community.jpeg</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Alexis Garza (@65251217)</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Juan Herrera (@12010452)</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>45348</v>
+      </c>
+      <c r="F25" s="2" t="n">
+        <v>45354</v>
+      </c>
+      <c r="G25" t="n">
+        <v>30</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Off firm approach top this mention trouble. Start newspaper lawyer when teach just entire. Try already coach discover fly.
+Special sit raise true. Middle ground candidate.</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>James Meyer</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>RECHAZADO - CONTABILIDAD</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Type 2</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>Juan Herrera (@12010452),Jasmine Abbott (@7142464)</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>listen.mp4</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Jonathan Hall (@81435130)</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Jasmine Abbott (@7142464)</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>45378</v>
+      </c>
+      <c r="F26" s="2" t="n">
+        <v>45379</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Strong sign different imagine eight own race. Yard work financial explain exactly everyone commercial word. Growth or million read.
+Walk main continue herself policy. Natural beyond room.</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Katherine Love</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>EN PROCESO</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Type 1</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>Denise Cunningham (@61472431),Juan Herrera (@12010452)</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>hot.webm</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Juan Herrera (@12010452)</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Jasmine Abbott (@7142464)</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>45375</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>45396</v>
+      </c>
+      <c r="G27" t="n">
+        <v>3</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Shake value show large admit. Human ahead figure trouble your.
+Thing which attention eat more. Major nor media every could. Without hour election value.</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Cheyenne Johnson</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>RECHAZADO - CONTABILIDAD</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Type 1</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>Jasmine Abbott (@7142464)</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>pay.js</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Brittany Martinez (@29904970)</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Juan Herrera (@12010452)</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>45357</v>
+      </c>
+      <c r="F28" s="2" t="n">
+        <v>45385</v>
+      </c>
+      <c r="G28" t="n">
+        <v>21</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Appear morning think thousand third major.
+Accept staff operation for admit magazine. Relationship ahead institution knowledge decade.
+Especially I character apply. Maintain rock car our he.</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Laura Smith</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>CERRADO</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Type 2</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>Jasmine Abbott (@7142464),Jasmine Abbott (@7142464)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>reason.pages</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Jodi Hansen (@21049704)</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Jasmine Abbott (@7142464)</t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>45354</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>45360</v>
+      </c>
+      <c r="G29" t="n">
+        <v>24</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Near manage cell various. Report she fast clear put training. Measure power safe. Enter begin manage letter sit trouble create.</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Kathryn Quinn</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>PAGADO - CONTABILIDAD</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>Type 3</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>Juan Herrera (@12010452),Jasmine Abbott (@7142464)</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>sign.avi</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Michelle Sandoval (@88258637)</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Jodi Hansen (@21049704)</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>45359</v>
+      </c>
+      <c r="F30" s="2" t="n">
+        <v>45374</v>
+      </c>
+      <c r="G30" t="n">
+        <v>19</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Affect professor guy standard my former. Level capital most those anyone occur.
+Bad stage language dream week build. Majority section many.
+Also management list town. Almost type board.</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Laura Alexander</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>RECHAZADO - CENCO</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>Type 2</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>Jasmine Abbott (@7142464)</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>possible.mp3</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Denise Cunningham (@61472431)</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Tyler Gomez (@51016002)</t>
+        </is>
+      </c>
+      <c r="E31" s="3" t="n">
+        <v>45370</v>
+      </c>
+      <c r="F31" s="3" t="n">
+        <v>45399</v>
+      </c>
+      <c r="G31" t="n">
+        <v>8</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Reflect house education low tonight later. Need law center before.
+Present need sort character force leave writer. Role others film sometimes any.</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Brian Flores</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>EN PROCESO</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>Type 3</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>Jasmine Abbott (@7142464),Juan Herrera (@12010452),Jonathan Hall (@81435130)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: changed api response to JsonResponse
</commit_message>
<xml_diff>
--- a/djangoproyect/static/requests/emulation/requests_database.xlsx
+++ b/djangoproyect/static/requests/emulation/requests_database.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,11 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-    <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="167" formatCode="YYYY-MM-DD"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -60,13 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -544,7 +541,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>EN PROCESO</t>
+          <t>APROBADO - DECANO</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -2116,10 +2113,10 @@
           <t>Tyler Gomez (@51016002)</t>
         </is>
       </c>
-      <c r="E31" s="3" t="n">
+      <c r="E31" s="2" t="n">
         <v>45370</v>
       </c>
-      <c r="F31" s="3" t="n">
+      <c r="F31" s="2" t="n">
         <v>45399</v>
       </c>
       <c r="G31" t="n">

</xml_diff>

<commit_message>
fix: Requests page not displaying after login
</commit_message>
<xml_diff>
--- a/djangoproyect/static/requests/emulation/requests_database.xlsx
+++ b/djangoproyect/static/requests/emulation/requests_database.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -541,7 +541,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>RECHAZADO - CONTABILIDAD</t>
+          <t>APROBADO - CENCO</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">

</xml_diff>

<commit_message>
feat: traceability model made
</commit_message>
<xml_diff>
--- a/djangoproyect/static/requests/emulation/requests_database.xlsx
+++ b/djangoproyect/static/requests/emulation/requests_database.xlsx
@@ -16,9 +16,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="167" formatCode="YYYY-MM-DD"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -58,12 +60,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2093,6 +2096,1101 @@
         </is>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>check.flac</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Heather Carrillo (@31725671)</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Robin Blair (@16670044)</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>45374</v>
+      </c>
+      <c r="F31" s="2" t="n">
+        <v>45377</v>
+      </c>
+      <c r="G31" t="n">
+        <v>5</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Skill pick find cell trouble method ten. Food later baby both. Ago us girl find. Laugh discover contain.</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Jamie Willis</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>RECHAZADO - CENCO</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>Type 1</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>Jon Palmer (@23400841),Heather Carrillo (@31725671),Jon Palmer (@23400841)</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>sound.flac</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Jennifer Fuentes (@9840607)</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Jon Palmer (@23400841)</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>45380</v>
+      </c>
+      <c r="F32" s="2" t="n">
+        <v>45399</v>
+      </c>
+      <c r="G32" t="n">
+        <v>-1</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Exactly activity agreement store program seem politics across. Ten commercial employee senior democratic region local. Benefit why collection feeling.</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Nathan Brown</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>RECHAZADO - CENCO</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>Type 2</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>Jon Palmer (@23400841),Jon Palmer (@23400841),Heather Carrillo (@31725671)</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>half.mov</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Heather Carrillo (@31725671)</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Melissa Cox (@51800599)</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>45368</v>
+      </c>
+      <c r="F33" s="2" t="n">
+        <v>45382</v>
+      </c>
+      <c r="G33" t="n">
+        <v>11</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Gas help region those walk everybody seek hair. Account measure such popular part. Book issue fill tough natural rest. Seven few necessary model direction contain.
+First about song begin.</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Nicole Hunter</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>RECHAZADO - DECANO</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>Type 3</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>Heather Carrillo (@31725671),Kim Rosales (@39851784)</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>commercial.xlsx</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Kevin Foster (@32273703)</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Kevin Foster (@32273703)</t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>45355</v>
+      </c>
+      <c r="F34" s="2" t="n">
+        <v>45356</v>
+      </c>
+      <c r="G34" t="n">
+        <v>24</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Hear current power field. Until little environmental clearly though decision. Win fast address million push financial. Huge best dinner situation.</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>Kimberly Hudson</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>CERRADO</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>Type 3</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>Heather Carrillo (@31725671),Jon Palmer (@23400841),Kim Rosales (@39851784)</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>page.jpeg</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Chad Fox (@44758173)</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Kim Rosales (@39851784)</t>
+        </is>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>45359</v>
+      </c>
+      <c r="F35" s="2" t="n">
+        <v>45386</v>
+      </c>
+      <c r="G35" t="n">
+        <v>20</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Walk tough industry pass radio world travel. Would finish PM Mr billion agency right. Camera exactly class identify.</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Brooke Oconnell</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>CERRADO</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>Type 1</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>Kim Rosales (@39851784),Jon Palmer (@23400841),Jon Palmer (@23400841)</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>TV.xlsx</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Kevin Foster (@32273703)</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Robin Blair (@16670044)</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>45369</v>
+      </c>
+      <c r="F36" s="2" t="n">
+        <v>45379</v>
+      </c>
+      <c r="G36" t="n">
+        <v>10</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>However quickly partner two yeah production into mother. Carry account near move this record. Third activity oil short.
+Laugh animal responsibility from technology.</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>Kristy Carney</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>APROBADO - CENCO</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>Type 2</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>Jon Palmer (@23400841),Jon Palmer (@23400841)</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>leg.xlsx</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Chad Fox (@44758173)</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Heather Carrillo (@31725671)</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>45353</v>
+      </c>
+      <c r="F37" s="2" t="n">
+        <v>45374</v>
+      </c>
+      <c r="G37" t="n">
+        <v>26</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Remember agreement later every sort south. Anything ready off research still night paper. Impact PM letter money since.</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>Jared Tucker</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>RECHAZADO - DECANO</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>Type 1</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>Kim Rosales (@39851784)</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>month.docx</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Melissa Cox (@51800599)</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Desiree Robinson (@58036467)</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>45372</v>
+      </c>
+      <c r="F38" s="2" t="n">
+        <v>45377</v>
+      </c>
+      <c r="G38" t="n">
+        <v>7</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Across new debate discussion least everybody. Decision reflect real painting throw operation.</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>Michael Huff</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>APROBADO - DECANO</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>Type 2</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>Heather Carrillo (@31725671)</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>week.jpeg</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Kevin Foster (@32273703)</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Heather Carrillo (@31725671)</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>45382</v>
+      </c>
+      <c r="F39" s="2" t="n">
+        <v>45383</v>
+      </c>
+      <c r="G39" t="n">
+        <v>-3</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Anything yet hope. Plan sing traditional fall. Finally even hotel agent discuss.
+Realize field wait simple.
+Most argue add protect fill business give. Commercial force never past.</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Willie Murphy</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>EN PROCESO</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>Type 3</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>Jon Palmer (@23400841),Jon Palmer (@23400841)</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>large.pages</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Desiree Robinson (@58036467)</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Chad Fox (@44758173)</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>45349</v>
+      </c>
+      <c r="F40" s="2" t="n">
+        <v>45357</v>
+      </c>
+      <c r="G40" t="n">
+        <v>30</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Collection total form family reduce power bank. Wide this culture production magazine drop.
+Party throw already its one expect until. Build drug certain always difference difference cut.</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Sarah Roberts</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>CERRADO</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>Type 3</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>Jon Palmer (@23400841),Jon Palmer (@23400841)</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>next.css</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Richard Thomas (@57640453)</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Melissa Johnson (@47666474)</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>45355</v>
+      </c>
+      <c r="F41" s="2" t="n">
+        <v>45370</v>
+      </c>
+      <c r="G41" t="n">
+        <v>24</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Movie young chair she off. Father serious painting positive voice become generation.
+Page ground too make everybody. Week subject able this back you. West international exist stand why authority one.</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Crystal Smith</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>RECHAZADO - CONTABILIDAD</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>Type 3</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>Melissa Johnson (@47666474)</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>apply.mp3</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Melissa Johnson (@47666474)</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Benjamin Miller (@1477097)</t>
+        </is>
+      </c>
+      <c r="E42" s="2" t="n">
+        <v>45381</v>
+      </c>
+      <c r="F42" s="2" t="n">
+        <v>45408</v>
+      </c>
+      <c r="G42" t="n">
+        <v>-2</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Thought military task another billion. Carry audience trouble apply.
+Education relate reach turn tell discover unit. Number only room ask.
+Interview record western scientist.</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>Jason Palmer</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>RECHAZADO - CENCO</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>Type 2</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>Melissa Johnson (@47666474),Taylor Wilkins (@5464236),Taylor Wilkins (@5464236)</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>author.js</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Melissa Johnson (@47666474)</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Melissa Johnson (@47666474)</t>
+        </is>
+      </c>
+      <c r="E43" s="2" t="n">
+        <v>45381</v>
+      </c>
+      <c r="F43" s="2" t="n">
+        <v>45382</v>
+      </c>
+      <c r="G43" t="n">
+        <v>-2</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Outside important we pull reveal early. Finally house crime region again poor.
+Magazine move who. Last hair human idea. Without part through president.</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>Melissa Johnson</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>RECHAZADO - CENCO</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>Type 2</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>Kenneth Chang (@59512309),Maria Lewis (@48114355)</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>case.mov</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Benjamin Miller (@1477097)</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Richard Thomas (@57640453)</t>
+        </is>
+      </c>
+      <c r="E44" s="2" t="n">
+        <v>45360</v>
+      </c>
+      <c r="F44" s="2" t="n">
+        <v>45376</v>
+      </c>
+      <c r="G44" t="n">
+        <v>19</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Author pick including able surface. Amount crime population develop clear late.
+Choose form argue more indicate contain. Pick example often entire. Course drive song good method.</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>Rachel Barton</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>APROBADO - CENCO</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>Type 3</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>Kenneth Chang (@59512309),Taylor Wilkins (@5464236),Taylor Wilkins (@5464236)</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>red.gif</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Shannon Brown (@90416220)</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Maria Lewis (@48114355)</t>
+        </is>
+      </c>
+      <c r="E45" s="2" t="n">
+        <v>45359</v>
+      </c>
+      <c r="F45" s="2" t="n">
+        <v>45360</v>
+      </c>
+      <c r="G45" t="n">
+        <v>20</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Network second serve arm. Full thank son send.
+Discover court after. Article yard when write music forget.
+Minute especially better people final. Third its nearly he. Hold scientist magazine walk.</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>Ryan Delacruz</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>RECHAZADO - DECANO</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>Type 1</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>Melissa Johnson (@47666474)</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Mrs.html</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Richard Thomas (@57640453)</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Benjamin Miller (@1477097)</t>
+        </is>
+      </c>
+      <c r="E46" s="2" t="n">
+        <v>45353</v>
+      </c>
+      <c r="F46" s="2" t="n">
+        <v>45360</v>
+      </c>
+      <c r="G46" t="n">
+        <v>26</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Data mean truth despite describe step arrive seven. A again job television.
+Yet smile forward like nice attack these. Mother card data wrong hand.</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>Vincent Guerra</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>RECHAZADO - CENCO</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>Type 1</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>Taylor Wilkins (@5464236),Maria Lewis (@48114355)</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>tend.mp4</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Melissa Johnson (@47666474)</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Maria Lewis (@48114355)</t>
+        </is>
+      </c>
+      <c r="E47" s="2" t="n">
+        <v>45373</v>
+      </c>
+      <c r="F47" s="2" t="n">
+        <v>45383</v>
+      </c>
+      <c r="G47" t="n">
+        <v>6</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Future political simple star. Seem see join vote condition continue. Lead phone bad collection.</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>Michael Dunn</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>CERRADO</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>Type 2</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>Melissa Johnson (@47666474),Kenneth Chang (@59512309)</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>last.pdf</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Julia Herman (@87635666)</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Julia Herman (@87635666)</t>
+        </is>
+      </c>
+      <c r="E48" s="2" t="n">
+        <v>45377</v>
+      </c>
+      <c r="F48" s="2" t="n">
+        <v>45406</v>
+      </c>
+      <c r="G48" t="n">
+        <v>2</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Indicate your series describe. Such imagine few control most. Economic behind security especially whole each rise fast.</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>Katelyn Harrell</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>EN PROCESO</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>Type 2</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>Maria Lewis (@48114355)</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>structure.mp3</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Shannon Brown (@90416220)</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Maria Lewis (@48114355)</t>
+        </is>
+      </c>
+      <c r="E49" s="2" t="n">
+        <v>45360</v>
+      </c>
+      <c r="F49" s="2" t="n">
+        <v>45376</v>
+      </c>
+      <c r="G49" t="n">
+        <v>19</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Structure ask region voice professional really cup. Suggest too hour economy career right.
+Perform TV else color. Box nation cut wonder often speak effort beautiful. Expect high each get baby do.</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Michael Johnston</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>APROBADO - CENCO</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>Type 1</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>Kenneth Chang (@59512309),Taylor Wilkins (@5464236)</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>program.flac</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Shannon Brown (@90416220)</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Kenneth Chang (@59512309)</t>
+        </is>
+      </c>
+      <c r="E50" s="3" t="n">
+        <v>45360</v>
+      </c>
+      <c r="F50" s="3" t="n">
+        <v>45380</v>
+      </c>
+      <c r="G50" t="n">
+        <v>19</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Major walk report community move green school.
+North no peace want term change brother. Education of class job hard example speak minute.</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>Jack Jackson</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>APROBADO - DECANO</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>Type 1</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>Taylor Wilkins (@5464236),Kenneth Chang (@59512309),Melissa Johnson (@47666474)</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>